<commit_message>
german tutorial on data collecting finished
</commit_message>
<xml_diff>
--- a/GitHubPages/documents/1_Lieferliste Caterer 1a.xlsx
+++ b/GitHubPages/documents/1_Lieferliste Caterer 1a.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stations" sheetId="1" r:id="rId1"/>
@@ -14,19 +14,19 @@
     <sheet name="Help" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="DeliveryIDs">Deliveries!$A$3:$A$13491</definedName>
+    <definedName name="DeliveryIDs">Deliveries!$A$3:$A$13467</definedName>
     <definedName name="Sampling">LookUp!$A$2:$A$13</definedName>
     <definedName name="StationIDs">Stations!$A$2:$A$945</definedName>
     <definedName name="ToB">LookUp!$B$2:$B$11</definedName>
     <definedName name="Treatment">LookUp!$C$2:$C$11</definedName>
     <definedName name="Units">LookUp!$D$2:$D$31</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="133">
   <si>
     <t>Company_ID</t>
   </si>
@@ -613,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -678,9 +678,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1129,7 +1126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1623,11 +1620,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK28"/>
+  <dimension ref="A1:AMK4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,73 +1658,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="35" t="s">
+      <c r="F1" s="36"/>
+      <c r="G1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="36" t="s">
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="37" t="s">
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="38" t="s">
+      <c r="N1" s="36"/>
+      <c r="O1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="Q1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="R1" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33" t="s">
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33" t="s">
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="Y1" s="34" t="s">
+      <c r="Y1" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
     </row>
     <row r="2" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="12" t="s">
         <v>64</v>
       </c>
@@ -1758,9 +1755,9 @@
       <c r="N2" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="33"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="32"/>
       <c r="R2" s="15" t="s">
         <v>66</v>
       </c>
@@ -1779,24 +1776,24 @@
       <c r="W2" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30"/>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
+      <c r="AE2" s="30"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
-        <f t="shared" ref="A3:A28" si="0">B3&amp;";"&amp;C3&amp;";"&amp;D3&amp;";"&amp;G3&amp;"."&amp;H3&amp;"."&amp;I3&amp;";"&amp;O3</f>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9001</v>
+        <f t="shared" ref="A3:A4" si="0">B3&amp;";"&amp;C3&amp;";"&amp;D3&amp;";"&amp;G3&amp;"."&amp;H3&amp;"."&amp;I3&amp;";"&amp;O3</f>
+        <v>3001asaa;Menü 1;M01;3.9.2014;9012</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1827,28 +1824,28 @@
         <v>2014</v>
       </c>
       <c r="M3" s="1">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="N3" s="11" t="s">
         <v>71</v>
       </c>
       <c r="O3" s="1">
-        <v>9001</v>
+        <v>9012</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9002</v>
+        <v>3001asaa;Menü 2;M02;3.9.2014;9008</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E4" s="1">
         <v>900</v>
@@ -1875,1165 +1872,13 @@
         <v>2014</v>
       </c>
       <c r="M4" s="1">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>71</v>
       </c>
       <c r="O4" s="1">
-        <v>9002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9003</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="1">
-        <v>900</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="1">
-        <v>3</v>
-      </c>
-      <c r="H5" s="1">
-        <v>9</v>
-      </c>
-      <c r="I5" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J5" s="1">
-        <v>3</v>
-      </c>
-      <c r="K5" s="1">
-        <v>9</v>
-      </c>
-      <c r="L5" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M5" s="1">
-        <v>68</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O5" s="1">
-        <v>9003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9004</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="1">
-        <v>900</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="1">
-        <v>3</v>
-      </c>
-      <c r="H6" s="1">
-        <v>9</v>
-      </c>
-      <c r="I6" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J6" s="1">
-        <v>3</v>
-      </c>
-      <c r="K6" s="1">
-        <v>9</v>
-      </c>
-      <c r="L6" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M6" s="1">
-        <v>29</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O6" s="1">
-        <v>9004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9005</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="1">
-        <v>900</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G7" s="1">
-        <v>3</v>
-      </c>
-      <c r="H7" s="1">
-        <v>9</v>
-      </c>
-      <c r="I7" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J7" s="1">
-        <v>3</v>
-      </c>
-      <c r="K7" s="1">
-        <v>9</v>
-      </c>
-      <c r="L7" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M7" s="1">
-        <v>46</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O7" s="1">
-        <v>9005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9006</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="1">
-        <v>900</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G8" s="1">
-        <v>3</v>
-      </c>
-      <c r="H8" s="1">
-        <v>9</v>
-      </c>
-      <c r="I8" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J8" s="1">
-        <v>3</v>
-      </c>
-      <c r="K8" s="1">
-        <v>9</v>
-      </c>
-      <c r="L8" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M8" s="1">
-        <v>48</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O8" s="1">
-        <v>9006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9007</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="1">
-        <v>900</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="1">
-        <v>3</v>
-      </c>
-      <c r="H9" s="1">
-        <v>9</v>
-      </c>
-      <c r="I9" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J9" s="1">
-        <v>3</v>
-      </c>
-      <c r="K9" s="1">
-        <v>9</v>
-      </c>
-      <c r="L9" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M9" s="1">
-        <v>45</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O9" s="1">
-        <v>9007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9008</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="1">
-        <v>900</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="1">
-        <v>3</v>
-      </c>
-      <c r="H10" s="1">
-        <v>9</v>
-      </c>
-      <c r="I10" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J10" s="1">
-        <v>3</v>
-      </c>
-      <c r="K10" s="1">
-        <v>9</v>
-      </c>
-      <c r="L10" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M10" s="1">
-        <v>50</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O10" s="1">
         <v>9008</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9009</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="1">
-        <v>900</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="1">
-        <v>3</v>
-      </c>
-      <c r="H11" s="1">
-        <v>9</v>
-      </c>
-      <c r="I11" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J11" s="1">
-        <v>3</v>
-      </c>
-      <c r="K11" s="1">
-        <v>9</v>
-      </c>
-      <c r="L11" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M11" s="1">
-        <v>38</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O11" s="1">
-        <v>9009</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9010</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="1">
-        <v>900</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" s="1">
-        <v>3</v>
-      </c>
-      <c r="H12" s="1">
-        <v>9</v>
-      </c>
-      <c r="I12" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J12" s="1">
-        <v>3</v>
-      </c>
-      <c r="K12" s="1">
-        <v>9</v>
-      </c>
-      <c r="L12" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M12" s="1">
-        <v>69</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O12" s="1">
-        <v>9010</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9011</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="1">
-        <v>900</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" s="1">
-        <v>3</v>
-      </c>
-      <c r="H13" s="1">
-        <v>9</v>
-      </c>
-      <c r="I13" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J13" s="1">
-        <v>3</v>
-      </c>
-      <c r="K13" s="1">
-        <v>9</v>
-      </c>
-      <c r="L13" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M13" s="1">
-        <v>60</v>
-      </c>
-      <c r="N13" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O13" s="1">
-        <v>9011</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9012</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="1">
-        <v>900</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="1">
-        <v>3</v>
-      </c>
-      <c r="H14" s="1">
-        <v>9</v>
-      </c>
-      <c r="I14" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J14" s="1">
-        <v>3</v>
-      </c>
-      <c r="K14" s="1">
-        <v>9</v>
-      </c>
-      <c r="L14" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M14" s="1">
-        <v>62</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O14" s="1">
-        <v>9012</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9013</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="1">
-        <v>900</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="1">
-        <v>3</v>
-      </c>
-      <c r="H15" s="1">
-        <v>9</v>
-      </c>
-      <c r="I15" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J15" s="1">
-        <v>3</v>
-      </c>
-      <c r="K15" s="1">
-        <v>9</v>
-      </c>
-      <c r="L15" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M15" s="1">
-        <v>77</v>
-      </c>
-      <c r="N15" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O15" s="1">
-        <v>9013</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9014</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="1">
-        <v>900</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="1">
-        <v>3</v>
-      </c>
-      <c r="H16" s="1">
-        <v>9</v>
-      </c>
-      <c r="I16" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J16" s="1">
-        <v>3</v>
-      </c>
-      <c r="K16" s="1">
-        <v>9</v>
-      </c>
-      <c r="L16" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M16" s="1">
-        <v>47</v>
-      </c>
-      <c r="N16" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O16" s="1">
-        <v>9014</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 1;M01;3.9.2014;9015</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="1">
-        <v>900</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="1">
-        <v>3</v>
-      </c>
-      <c r="H17" s="1">
-        <v>9</v>
-      </c>
-      <c r="I17" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J17" s="1">
-        <v>3</v>
-      </c>
-      <c r="K17" s="1">
-        <v>9</v>
-      </c>
-      <c r="L17" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M17" s="1">
-        <v>40</v>
-      </c>
-      <c r="N17" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O17" s="1">
-        <v>9015</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 2;M02;3.9.2014;9001</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1200</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G18" s="1">
-        <v>3</v>
-      </c>
-      <c r="H18" s="1">
-        <v>9</v>
-      </c>
-      <c r="I18" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J18" s="1">
-        <v>3</v>
-      </c>
-      <c r="K18" s="1">
-        <v>9</v>
-      </c>
-      <c r="L18" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M18" s="1">
-        <v>77</v>
-      </c>
-      <c r="N18" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O18" s="1">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 2;M02;3.9.2014;9002</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1200</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="1">
-        <v>3</v>
-      </c>
-      <c r="H19" s="1">
-        <v>9</v>
-      </c>
-      <c r="I19" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J19" s="1">
-        <v>3</v>
-      </c>
-      <c r="K19" s="1">
-        <v>9</v>
-      </c>
-      <c r="L19" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M19" s="1">
-        <v>89</v>
-      </c>
-      <c r="N19" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O19" s="1">
-        <v>9002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 2;M02;3.9.2014;9007</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1200</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" s="1">
-        <v>3</v>
-      </c>
-      <c r="H20" s="1">
-        <v>9</v>
-      </c>
-      <c r="I20" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J20" s="1">
-        <v>3</v>
-      </c>
-      <c r="K20" s="1">
-        <v>9</v>
-      </c>
-      <c r="L20" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M20" s="1">
-        <v>82</v>
-      </c>
-      <c r="N20" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O20" s="1">
-        <v>9007</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 2;M02;3.9.2014;9008</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1200</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="1">
-        <v>3</v>
-      </c>
-      <c r="H21" s="1">
-        <v>9</v>
-      </c>
-      <c r="I21" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J21" s="1">
-        <v>3</v>
-      </c>
-      <c r="K21" s="1">
-        <v>9</v>
-      </c>
-      <c r="L21" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M21" s="1">
-        <v>101</v>
-      </c>
-      <c r="N21" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O21" s="1">
-        <v>9008</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 2;M02;3.9.2014;9009</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="1">
-        <v>1200</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="1">
-        <v>3</v>
-      </c>
-      <c r="H22" s="1">
-        <v>9</v>
-      </c>
-      <c r="I22" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J22" s="1">
-        <v>3</v>
-      </c>
-      <c r="K22" s="1">
-        <v>9</v>
-      </c>
-      <c r="L22" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M22" s="1">
-        <v>50</v>
-      </c>
-      <c r="N22" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O22" s="1">
-        <v>9009</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 2;M02;3.9.2014;9010</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1200</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="1">
-        <v>3</v>
-      </c>
-      <c r="H23" s="1">
-        <v>9</v>
-      </c>
-      <c r="I23" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J23" s="1">
-        <v>3</v>
-      </c>
-      <c r="K23" s="1">
-        <v>9</v>
-      </c>
-      <c r="L23" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M23" s="1">
-        <v>77</v>
-      </c>
-      <c r="N23" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O23" s="1">
-        <v>9010</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 2;M02;3.9.2014;9011</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1200</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="1">
-        <v>3</v>
-      </c>
-      <c r="H24" s="1">
-        <v>9</v>
-      </c>
-      <c r="I24" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J24" s="1">
-        <v>3</v>
-      </c>
-      <c r="K24" s="1">
-        <v>9</v>
-      </c>
-      <c r="L24" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M24" s="1">
-        <v>78</v>
-      </c>
-      <c r="N24" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O24" s="1">
-        <v>9011</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 2;M02;3.9.2014;9012</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1200</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="1">
-        <v>3</v>
-      </c>
-      <c r="H25" s="1">
-        <v>9</v>
-      </c>
-      <c r="I25" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J25" s="1">
-        <v>3</v>
-      </c>
-      <c r="K25" s="1">
-        <v>9</v>
-      </c>
-      <c r="L25" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M25" s="1">
-        <v>62</v>
-      </c>
-      <c r="N25" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O25" s="1">
-        <v>9012</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 2;M02;3.9.2014;9013</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1200</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G26" s="1">
-        <v>3</v>
-      </c>
-      <c r="H26" s="1">
-        <v>9</v>
-      </c>
-      <c r="I26" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J26" s="1">
-        <v>3</v>
-      </c>
-      <c r="K26" s="1">
-        <v>9</v>
-      </c>
-      <c r="L26" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M26" s="1">
-        <v>73</v>
-      </c>
-      <c r="N26" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O26" s="1">
-        <v>9013</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 2;M02;3.9.2014;9014</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1200</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="1">
-        <v>3</v>
-      </c>
-      <c r="H27" s="1">
-        <v>9</v>
-      </c>
-      <c r="I27" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J27" s="1">
-        <v>3</v>
-      </c>
-      <c r="K27" s="1">
-        <v>9</v>
-      </c>
-      <c r="L27" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M27" s="1">
-        <v>112</v>
-      </c>
-      <c r="N27" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O27" s="1">
-        <v>9014</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3001asaa;Menü 2;M02;3.9.2014;9015</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="1">
-        <v>1200</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G28" s="1">
-        <v>3</v>
-      </c>
-      <c r="H28" s="1">
-        <v>9</v>
-      </c>
-      <c r="I28" s="1">
-        <v>2014</v>
-      </c>
-      <c r="J28" s="1">
-        <v>3</v>
-      </c>
-      <c r="K28" s="1">
-        <v>9</v>
-      </c>
-      <c r="L28" s="1">
-        <v>2014</v>
-      </c>
-      <c r="M28" s="1">
-        <v>40</v>
-      </c>
-      <c r="N28" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O28" s="1">
-        <v>9015</v>
       </c>
     </row>
   </sheetData>
@@ -3061,51 +1906,51 @@
     <mergeCell ref="AD1:AD2"/>
   </mergeCells>
   <dataValidations count="12">
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E18:E28">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="E3 M3:M4">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="E3:E17 M3:M28">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U3:U28 R3:R28">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R4 U3:U4">
       <formula1>1</formula1>
       <formula2>31</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3:V28 S3:S28">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3:S4 V3:V4">
       <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3:W28 T3:T28">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3:T4 W3:W4">
       <formula1>1900</formula1>
       <formula2>3000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" sqref="J3:J28 G3:G28">
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" sqref="G3:G4 J3:J4">
       <formula1>1</formula1>
       <formula2>31</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" sqref="K3:K28 H3:H28">
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" sqref="H3:H4 K3:K4">
       <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" sqref="L3:L28 I3:I28">
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" sqref="I3:I4 L3:L4">
       <formula1>1900</formula1>
       <formula2>3000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X3:X28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X3:X4">
       <formula1>Treatment</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y4">
       <formula1>Sampling</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N28 F3:F28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F4 N3:N4">
       <formula1>Units</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3:O28 B3:B28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4 O3:O4">
       <formula1>StationIDs</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3125,15 +1970,15 @@
   <cols>
     <col min="1" max="1" width="34.140625"/>
     <col min="2" max="2" width="35"/>
-    <col min="3" max="3" width="11.42578125" style="19"/>
+    <col min="3" max="3" width="11.42578125" style="18"/>
     <col min="4" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:9" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>75</v>
       </c>
       <c r="C1" s="8" t="s">
@@ -3149,13 +1994,13 @@
       <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3185,21 +2030,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3213,7 +2058,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>86</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -3241,7 +2086,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="1" t="s">
         <v>89</v>
       </c>
@@ -3265,7 +2110,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="1" t="s">
         <v>96</v>
       </c>
@@ -3310,7 +2155,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="26"/>
       <c r="C11" s="1" t="s">
         <v>107</v>
       </c>
@@ -3319,13 +2164,13 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="26"/>
       <c r="D12" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="26"/>
       <c r="D13" s="11" t="s">
         <v>110</v>
       </c>
@@ -3396,27 +2241,27 @@
       </c>
     </row>
     <row r="27" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="27" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="28" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="27" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="29" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="27" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="30" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="27" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="31" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="27" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3446,13 +2291,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>128</v>
       </c>
       <c r="B1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="29" t="s">
         <v>129</v>
       </c>
       <c r="B2" s="1" t="s">

</xml_diff>